<commit_message>
se realizo mas excepciones
</commit_message>
<xml_diff>
--- a/planilla_carga.xlsx
+++ b/planilla_carga.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="331">
   <si>
     <t>ID</t>
   </si>
@@ -936,6 +936,75 @@
   </si>
   <si>
     <t>896412.2509076085</t>
+  </si>
+  <si>
+    <t>82560</t>
+  </si>
+  <si>
+    <t>775571623</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>Aspiradora||Pan</t>
+  </si>
+  <si>
+    <t>985349.2435178054</t>
+  </si>
+  <si>
+    <t>43963</t>
+  </si>
+  <si>
+    <t>998705680</t>
+  </si>
+  <si>
+    <t>Isabel</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Cepillo de dientes</t>
+  </si>
+  <si>
+    <t>375302.89530345425</t>
+  </si>
+  <si>
+    <t>79471</t>
+  </si>
+  <si>
+    <t>578927681</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Batidora||Horno</t>
+  </si>
+  <si>
+    <t>ELECTRODOMESTICO||ELECTRODOMESTICO</t>
+  </si>
+  <si>
+    <t>650772.6144401672</t>
+  </si>
+  <si>
+    <t>91054</t>
+  </si>
+  <si>
+    <t>714860768</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>719233.2007133622</t>
   </si>
 </sst>
 </file>
@@ -980,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2687,6 +2756,170 @@
         <v>78</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F43" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="G43" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="H43" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="I43" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="J43" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="K43" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="L43" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="M43" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="H44" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="I44" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="J44" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="K44" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="L44" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="M44" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>320</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="G45" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="H45" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="I45" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="J45" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="K45" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="L45" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="M45" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="G46" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="H46" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="I46" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J46" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="K46" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="L46" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="M46" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>